<commit_message>
please dont change this any more
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmylim/Desktop/Bootcamp/R-Workshop-Day-1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/mock_thesis-master/R-Workshop-Day-1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9599AD-3D1F-6C44-86C7-96B6252FAB42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8826B1A1-C33D-C441-B086-ACA1CBB79755}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="13120" windowHeight="6100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="34">
   <si>
     <t>Petal.Width</t>
   </si>
@@ -4210,10 +4210,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4800,14 +4800,6 @@
       </c>
       <c r="B75" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>123</v>
-      </c>
-      <c r="B76" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>